<commit_message>
added and started protocol for testing
</commit_message>
<xml_diff>
--- a/data/Micropipette Presentation.xlsx
+++ b/data/Micropipette Presentation.xlsx
@@ -9,15 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9885" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9885" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Drift Test" sheetId="1" r:id="rId1"/>
-    <sheet name="200uL" sheetId="2" r:id="rId2"/>
-    <sheet name="50uL" sheetId="4" r:id="rId3"/>
-    <sheet name="20uL" sheetId="3" r:id="rId4"/>
-    <sheet name="10uL" sheetId="6" r:id="rId5"/>
-    <sheet name="Percent Error" sheetId="5" r:id="rId6"/>
+    <sheet name="Commercial Drift Test" sheetId="8" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId3"/>
+    <sheet name="200uL" sheetId="2" r:id="rId4"/>
+    <sheet name="50uL" sheetId="4" r:id="rId5"/>
+    <sheet name="20uL" sheetId="3" r:id="rId6"/>
+    <sheet name="10uL" sheetId="6" r:id="rId7"/>
+    <sheet name="Percent Error" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
   <si>
     <t>Amount Dispensed Experimental (1mL)Pipette (g)</t>
   </si>
@@ -83,6 +85,18 @@
   </si>
   <si>
     <t>10uL</t>
+  </si>
+  <si>
+    <t>Trial</t>
+  </si>
+  <si>
+    <t>Normal Distribution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean </t>
+  </si>
+  <si>
+    <t>Standard Error</t>
   </si>
 </sst>
 </file>
@@ -189,13 +203,7 @@
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -208,6 +216,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -573,11 +587,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1163613392"/>
-        <c:axId val="1163605232"/>
+        <c:axId val="1485888768"/>
+        <c:axId val="1485886048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1163613392"/>
+        <c:axId val="1485888768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -694,12 +708,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1163605232"/>
+        <c:crossAx val="1485886048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1163605232"/>
+        <c:axId val="1485886048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.19000000000000003"/>
@@ -818,7 +832,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1163613392"/>
+        <c:crossAx val="1485888768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1278,11 +1292,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1163610128"/>
-        <c:axId val="1163613936"/>
+        <c:axId val="1485884960"/>
+        <c:axId val="1485892576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1163610128"/>
+        <c:axId val="1485884960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1339,12 +1353,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1163613936"/>
+        <c:crossAx val="1485892576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1163613936"/>
+        <c:axId val="1485892576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1401,7 +1415,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1163610128"/>
+        <c:crossAx val="1485884960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1793,11 +1807,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1163603600"/>
-        <c:axId val="1163608496"/>
+        <c:axId val="1485881152"/>
+        <c:axId val="1485893120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1163603600"/>
+        <c:axId val="1485881152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1896,7 +1910,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1163608496"/>
+        <c:crossAx val="1485893120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1904,7 +1918,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1163608496"/>
+        <c:axId val="1485893120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2071,7 +2085,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1163603600"/>
+        <c:crossAx val="1485881152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4680,6 +4694,675 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="39.85546875" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0.2024</v>
+      </c>
+      <c r="D2">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>2.6467716594465577E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>0.20469999999999999</v>
+      </c>
+      <c r="D3">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.9483019129741338</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>0.2039</v>
+      </c>
+      <c r="D4">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.53672459929969107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>0.2046</v>
+      </c>
+      <c r="D5">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.9245776997255033</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>0.20369999999999999</v>
+      </c>
+      <c r="D6">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.38517382701143299</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>0.2044</v>
+      </c>
+      <c r="D7">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.85370321699152318</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>0.20469999999999999</v>
+      </c>
+      <c r="D8">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.9483019129741338</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>0.2044</v>
+      </c>
+      <c r="D9">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.85370321699152318</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="D10">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>5.0889513802385419E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>0.2031</v>
+      </c>
+      <c r="D11">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>7.4336205397422292E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="D12">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.61188602866781583</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>0.2041</v>
+      </c>
+      <c r="D13">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.68306639754315768</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>0.2049</v>
+      </c>
+      <c r="D14">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.97792757492818794</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>0.2041</v>
+      </c>
+      <c r="D15">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.68306639754315768</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>0.2039</v>
+      </c>
+      <c r="D16">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.53672459929969107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>0.20419999999999999</v>
+      </c>
+      <c r="D17">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.74804284607538918</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>0.20430000000000001</v>
+      </c>
+      <c r="D18">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.8052146928959476</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>0.20380000000000001</v>
+      </c>
+      <c r="D19">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.46022478711426418</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>0.20430000000000001</v>
+      </c>
+      <c r="D20">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.8052146928959476</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>0.20380000000000001</v>
+      </c>
+      <c r="D21">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.46022478711426418</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>0.2039</v>
+      </c>
+      <c r="D22">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.53672459929969107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>0.20380000000000001</v>
+      </c>
+      <c r="D23">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.46022478711426418</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>0.2036</v>
+      </c>
+      <c r="D24">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.31420254053967234</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>0.2041</v>
+      </c>
+      <c r="D25">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.68306639754315768</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>0.20319999999999999</v>
+      </c>
+      <c r="D26">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.10525142539243772</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>0.20269999999999999</v>
+      </c>
+      <c r="D27">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>1.346787383407707E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <v>0.2039</v>
+      </c>
+      <c r="D28">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.53672459929969107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="D29">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.61188602866781583</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <v>0.2031</v>
+      </c>
+      <c r="D30">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>7.4336205397422292E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>0.20419999999999999</v>
+      </c>
+      <c r="D31">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.74804284607538918</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <v>0.2039</v>
+      </c>
+      <c r="D32">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.53672459929969107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <v>0.20380000000000001</v>
+      </c>
+      <c r="D33">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.46022478711426418</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>0.2036</v>
+      </c>
+      <c r="D34">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.31420254053967234</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <v>0.2046</v>
+      </c>
+      <c r="D35">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.9245776997255033</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <v>0.2034</v>
+      </c>
+      <c r="D36">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.19267569947363233</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <v>0.20319999999999999</v>
+      </c>
+      <c r="D37">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.10525142539243772</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="C38">
+        <v>0.20369999999999999</v>
+      </c>
+      <c r="D38">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.38517382701143299</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="C39">
+        <v>0.2034</v>
+      </c>
+      <c r="D39">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.19267569947363233</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="C40">
+        <v>0.2034</v>
+      </c>
+      <c r="D40">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.19267569947363233</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="C41">
+        <v>0.20419999999999999</v>
+      </c>
+      <c r="D41">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.74804284607538918</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="C42">
+        <v>0.2041</v>
+      </c>
+      <c r="D42">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.68306639754315768</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="C43">
+        <v>0.2039</v>
+      </c>
+      <c r="D43">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.53672459929969107</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="C44">
+        <v>0.20380000000000001</v>
+      </c>
+      <c r="D44">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.46022478711426418</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="C45">
+        <v>0.2034</v>
+      </c>
+      <c r="D45">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.19267569947363233</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="C46">
+        <v>0.20449999999999999</v>
+      </c>
+      <c r="D46">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.89334253477604819</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="C47">
+        <v>0.20330000000000001</v>
+      </c>
+      <c r="D47">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.14454246253646461</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="C48">
+        <v>0.2039</v>
+      </c>
+      <c r="D48">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.53672459929969107</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="C49">
+        <v>0.20369999999999999</v>
+      </c>
+      <c r="D49">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.38517382701143299</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>0.2041</v>
+      </c>
+      <c r="D50">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.68306639754315768</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="C51">
+        <v>0.2039</v>
+      </c>
+      <c r="D51">
+        <f>NORMDIST(C:C,C54,C55,TRUE )</f>
+        <v>0.53672459929969107</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>20</v>
+      </c>
+      <c r="C54">
+        <f>AVERAGE(C2:C51)</f>
+        <v>0.20385200000000009</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>2</v>
+      </c>
+      <c r="C55">
+        <f>STDEV(C2:C51)</f>
+        <v>5.2069027967395216E-4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>21</v>
+      </c>
+      <c r="C56">
+        <f>(C55/(SQRT(50)))</f>
+        <v>7.3636725531074304E-5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4865,7 +5548,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
@@ -5053,7 +5736,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
@@ -5240,12 +5923,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="H7:K11"/>
+      <selection activeCell="B1" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5254,168 +5937,168 @@
     <col min="3" max="3" width="33.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="3">
         <v>9.7000000000000003E-3</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="3">
         <v>1.01E-2</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="3">
         <v>9.7999999999999997E-3</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="3">
         <v>1.0500000000000001E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
+      <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="3">
         <v>9.4999999999999998E-3</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <v>1.0699999999999999E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
+      <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="3">
         <v>9.4999999999999998E-3</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <v>1.01E-2</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="3">
         <v>9.1000000000000004E-3</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="3">
         <v>1.03E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="3">
         <v>9.9000000000000008E-3</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="3">
         <v>1.06E-2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+      <c r="A9" s="5">
         <v>7</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="6">
         <v>9.5999999999999992E-3</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="6">
         <v>1.01E-2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="5">
         <v>8</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="6">
         <v>9.7999999999999997E-3</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="6">
         <v>1.01E-2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="A11" s="5">
         <v>9</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="6">
         <v>9.9000000000000008E-3</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="6">
         <v>1.03E-2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="A12" s="5">
         <v>10</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="6">
         <v>9.7999999999999997E-3</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="6">
         <v>1.0200000000000001E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+      <c r="A13" s="5">
         <v>11</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="6">
         <v>1.01E-2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+      <c r="A14" s="5">
         <v>12</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="6">
         <v>9.7999999999999997E-3</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+      <c r="A15" s="5">
         <v>13</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="6">
         <v>1.03E-2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
+      <c r="A16" s="5">
         <v>14</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="6">
         <v>9.7999999999999997E-3</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
+      <c r="A17" s="5">
         <v>15</v>
       </c>
     </row>
@@ -5480,11 +6163,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
started user-data analysis, started luerlock fix
</commit_message>
<xml_diff>
--- a/data/Micropipette Presentation.xlsx
+++ b/data/Micropipette Presentation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9885" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9885" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Drift Test" sheetId="1" r:id="rId1"/>
@@ -587,11 +587,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1485888768"/>
-        <c:axId val="1485886048"/>
+        <c:axId val="334244000"/>
+        <c:axId val="334246720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1485888768"/>
+        <c:axId val="334244000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -708,12 +708,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1485886048"/>
+        <c:crossAx val="334246720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1485886048"/>
+        <c:axId val="334246720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.19000000000000003"/>
@@ -832,7 +832,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1485888768"/>
+        <c:crossAx val="334244000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1292,11 +1292,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1485884960"/>
-        <c:axId val="1485892576"/>
+        <c:axId val="333855856"/>
+        <c:axId val="333865648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1485884960"/>
+        <c:axId val="333855856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1353,12 +1353,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1485892576"/>
+        <c:crossAx val="333865648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1485892576"/>
+        <c:axId val="333865648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1415,7 +1415,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1485884960"/>
+        <c:crossAx val="333855856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1509,7 +1509,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1610,7 +1609,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1735,7 +1733,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1807,11 +1804,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1485881152"/>
-        <c:axId val="1485893120"/>
+        <c:axId val="333852592"/>
+        <c:axId val="333856400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1485881152"/>
+        <c:axId val="333852592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1843,7 +1840,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1910,7 +1906,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1485893120"/>
+        <c:crossAx val="333856400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1918,7 +1914,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1485893120"/>
+        <c:axId val="333856400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2010,7 +2006,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2085,7 +2080,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1485881152"/>
+        <c:crossAx val="333852592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4696,7 +4691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -5365,7 +5360,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -5553,7 +5548,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="A18:C21"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>